<commit_message>
Overvalued by ~14%, plus coffee overrated. WOuld need P to drop
</commit_message>
<xml_diff>
--- a/SBUX.xlsx
+++ b/SBUX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameelbrannon/Dropbox/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D2770E-A275-084D-822B-DB247B600A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6559ABE9-A7E8-AE49-9DDE-4921AEDFFA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10540" yWindow="780" windowWidth="43040" windowHeight="24560" activeTab="1" xr2:uid="{39773B44-95BC-A641-A327-344C16B2EF1F}"/>
+    <workbookView xWindow="1760" yWindow="640" windowWidth="43040" windowHeight="24560" activeTab="1" xr2:uid="{39773B44-95BC-A641-A327-344C16B2EF1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -886,12 +886,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -971,7 +977,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1033,15 +1039,16 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1049,7 +1056,18 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1067,15 +1085,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>392490</xdr:colOff>
+      <xdr:colOff>547688</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>16933</xdr:rowOff>
+      <xdr:rowOff>1058</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>169131</xdr:colOff>
+      <xdr:colOff>2443</xdr:colOff>
       <xdr:row>181</xdr:row>
-      <xdr:rowOff>71119</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1090,8 +1108,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="12228890" y="16933"/>
-          <a:ext cx="276174" cy="26546386"/>
+          <a:off x="12342813" y="1058"/>
+          <a:ext cx="10380" cy="26113317"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1122,13 +1140,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
+      <xdr:colOff>547687</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>501952</xdr:colOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>1890</xdr:colOff>
       <xdr:row>180</xdr:row>
       <xdr:rowOff>95673</xdr:rowOff>
     </xdr:to>
@@ -1145,8 +1163,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="19629059" y="0"/>
-          <a:ext cx="25703" cy="26052054"/>
+          <a:off x="19851687" y="0"/>
+          <a:ext cx="25703" cy="25940173"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1477,7 +1495,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="270" zoomScaleNormal="270" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -1510,7 +1528,7 @@
         <v>12</v>
       </c>
       <c r="I7" s="4">
-        <v>92.37</v>
+        <v>99.56</v>
       </c>
       <c r="L7" s="8"/>
     </row>
@@ -1531,7 +1549,7 @@
       </c>
       <c r="I9" s="4">
         <f>+I7*I8</f>
-        <v>107010.645</v>
+        <v>115340.26000000001</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1572,7 +1590,7 @@
       </c>
       <c r="I12" s="2">
         <f>+I9-I10+I11</f>
-        <v>118592.545</v>
+        <v>126922.16</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1606,9 +1624,6 @@
       <c r="C16" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="I16" s="4">
-        <v>400</v>
-      </c>
     </row>
     <row r="17" spans="2:9">
       <c r="B17" s="16">
@@ -1617,17 +1632,11 @@
       <c r="C17" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="I17" s="4">
-        <v>344.97</v>
-      </c>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" s="17"/>
       <c r="C18" s="8"/>
-      <c r="I18" s="8">
-        <f>+I16/I17-1</f>
-        <v>0.15952111777835754</v>
-      </c>
+      <c r="I18" s="8"/>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="17"/>
@@ -1698,10 +1707,10 @@
   <dimension ref="B2:IL173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="N63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AB18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V72" sqref="V72"/>
+      <selection pane="bottomRight" activeCell="AQ53" sqref="AQ53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" outlineLevelRow="1"/>
@@ -1719,7 +1728,8 @@
     <col min="26" max="28" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="29" max="31" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="37" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="48" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="48" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="8.5" style="4" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="7.5" style="4" bestFit="1" customWidth="1"/>
@@ -5153,44 +5163,44 @@
         <v>97</v>
       </c>
       <c r="AM38" s="4">
-        <f>+AM34*(AL38/AL34)</f>
-        <v>138.80559721073243</v>
+        <f>+AM58*$AY$47</f>
+        <v>117.24544000000002</v>
       </c>
       <c r="AN38" s="4">
-        <f>+AN34*(AM38/AM34)</f>
-        <v>149.59576816371782</v>
+        <f t="shared" ref="AN38:AV38" si="67">+AN58*$AY$47</f>
+        <v>121.93525760000003</v>
       </c>
       <c r="AO38" s="4">
-        <f t="shared" ref="AO38:AV38" si="67">+AO34*(AN38/AN34)</f>
-        <v>160.76202371593828</v>
+        <f t="shared" si="67"/>
+        <v>126.81266790400004</v>
       </c>
       <c r="AP38" s="4">
         <f t="shared" si="67"/>
-        <v>172.31509118298192</v>
+        <v>131.88517462016003</v>
       </c>
       <c r="AQ38" s="4">
         <f t="shared" si="67"/>
-        <v>184.26597653922107</v>
+        <v>137.16058160496644</v>
       </c>
       <c r="AR38" s="4">
         <f t="shared" si="67"/>
-        <v>196.62597127323647</v>
+        <v>142.6470048691651</v>
       </c>
       <c r="AS38" s="4">
         <f t="shared" si="67"/>
-        <v>209.40665940599678</v>
+        <v>148.35288506393172</v>
       </c>
       <c r="AT38" s="4">
         <f t="shared" si="67"/>
-        <v>222.61992467555839</v>
+        <v>154.28700046648899</v>
       </c>
       <c r="AU38" s="4">
         <f t="shared" si="67"/>
-        <v>236.27795789214008</v>
+        <v>160.45848048514856</v>
       </c>
       <c r="AV38" s="4">
         <f t="shared" si="67"/>
-        <v>250.39326446751477</v>
+        <v>166.87681970455452</v>
       </c>
     </row>
     <row r="39" spans="2:246">
@@ -5292,43 +5302,43 @@
         <v>-482.8</v>
       </c>
       <c r="AM39" s="4">
-        <f t="shared" ref="AM39:AV39" si="68">-SUM(AL80,AL83)*$AY$48</f>
+        <f>-SUM(AL80,AL83)*$AY$48</f>
         <v>-401.18132999999995</v>
       </c>
       <c r="AN39" s="4">
-        <f t="shared" si="68"/>
+        <f>-SUM(AM80,AM83)*$AY$48</f>
         <v>-389.14589009999997</v>
       </c>
       <c r="AO39" s="4">
-        <f t="shared" si="68"/>
+        <f>-SUM(AN80,AN83)*$AY$48</f>
         <v>-377.47151339700002</v>
       </c>
       <c r="AP39" s="4">
-        <f t="shared" si="68"/>
+        <f>-SUM(AO80,AO83)*$AY$48</f>
         <v>-366.14736799509001</v>
       </c>
       <c r="AQ39" s="4">
-        <f t="shared" si="68"/>
+        <f>-SUM(AP80,AP83)*$AY$48</f>
         <v>-355.16294695523732</v>
       </c>
       <c r="AR39" s="4">
-        <f t="shared" si="68"/>
+        <f>-SUM(AQ80,AQ83)*$AY$48</f>
         <v>-344.50805854658017</v>
       </c>
       <c r="AS39" s="4">
-        <f t="shared" si="68"/>
+        <f>-SUM(AR80,AR83)*$AY$48</f>
         <v>-334.17281679018276</v>
       </c>
       <c r="AT39" s="4">
-        <f t="shared" si="68"/>
+        <f t="shared" ref="AN39:AV39" si="68">-SUM(AS80,AS83)*$AY$48</f>
         <v>-324.14763228647729</v>
       </c>
       <c r="AU39" s="4">
-        <f t="shared" si="68"/>
+        <f>-SUM(AT80,AT83)*$AY$48</f>
         <v>-314.42320331788295</v>
       </c>
       <c r="AV39" s="4">
-        <f t="shared" si="68"/>
+        <f>-SUM(AU80,AU83)*$AY$48</f>
         <v>-304.99050721834652</v>
       </c>
     </row>
@@ -5458,43 +5468,43 @@
       </c>
       <c r="AM40" s="6">
         <f>+SUM(AM34:AM39)</f>
-        <v>6345.4861872107213</v>
+        <v>6323.9260299999887</v>
       </c>
       <c r="AN40" s="6">
         <f t="shared" ref="AN40:AU40" si="76">+SUM(AN34:AN39)</f>
-        <v>6881.9795548637148</v>
+        <v>6854.3190442999967</v>
       </c>
       <c r="AO40" s="6">
         <f t="shared" si="76"/>
-        <v>7436.3915094229378</v>
+        <v>7402.4421536109994</v>
       </c>
       <c r="AP40" s="6">
         <f t="shared" si="76"/>
-        <v>8009.2542856173277</v>
+        <v>7968.824369054506</v>
       </c>
       <c r="AQ40" s="6">
         <f t="shared" si="76"/>
-        <v>8601.1133374722413</v>
+        <v>8554.0079425379863</v>
       </c>
       <c r="AR40" s="6">
         <f t="shared" si="76"/>
-        <v>9212.5276812671091</v>
+        <v>9158.5487148630364</v>
       </c>
       <c r="AS40" s="6">
         <f t="shared" si="76"/>
-        <v>9844.0702461113924</v>
+        <v>9783.0164717693278</v>
       </c>
       <c r="AT40" s="6">
         <f t="shared" si="76"/>
-        <v>10496.328232330585</v>
+        <v>10427.995308121515</v>
       </c>
       <c r="AU40" s="6">
         <f t="shared" si="76"/>
-        <v>11169.903477858123</v>
+        <v>11094.084000451132</v>
       </c>
       <c r="AV40" s="6">
         <f t="shared" ref="AV40" si="77">+SUM(AV34:AV39)</f>
-        <v>11865.412832833113</v>
+        <v>11781.896388070152</v>
       </c>
     </row>
     <row r="41" spans="2:246">
@@ -5597,43 +5607,43 @@
       </c>
       <c r="AM41" s="4">
         <f>+AM40*(AL41/AL40)</f>
-        <v>1422.3701404069311</v>
+        <v>1417.5373312360857</v>
       </c>
       <c r="AN41" s="4">
         <f t="shared" ref="AN41:AV41" si="78">+AN40*(AM41/AM40)</f>
-        <v>1542.6276154313007</v>
+        <v>1536.427383781039</v>
       </c>
       <c r="AO41" s="4">
         <f t="shared" si="78"/>
-        <v>1666.9016247639595</v>
+        <v>1659.2917193022984</v>
       </c>
       <c r="AP41" s="4">
         <f t="shared" si="78"/>
-        <v>1795.3114712863251</v>
+        <v>1786.2489180947346</v>
       </c>
       <c r="AQ41" s="4">
         <f t="shared" si="78"/>
-        <v>1927.9794210463788</v>
+        <v>1917.4205284367629</v>
       </c>
       <c r="AR41" s="4">
         <f t="shared" si="78"/>
-        <v>2065.0307801342142</v>
+        <v>2052.9311446204019</v>
       </c>
       <c r="AS41" s="4">
         <f t="shared" si="78"/>
-        <v>2206.5939732652632</v>
+        <v>2192.9084867601759</v>
       </c>
       <c r="AT41" s="4">
         <f t="shared" si="78"/>
-        <v>2352.8006241141788</v>
+        <v>2337.4834824272962</v>
       </c>
       <c r="AU41" s="4">
         <f t="shared" si="78"/>
-        <v>2503.7856374432799</v>
+        <v>2486.7903501566552</v>
       </c>
       <c r="AV41" s="4">
         <f t="shared" si="78"/>
-        <v>2659.6872830703687</v>
+        <v>2640.9666848751981</v>
       </c>
     </row>
     <row r="42" spans="2:246">
@@ -5762,43 +5772,43 @@
       </c>
       <c r="AM42" s="4">
         <f>+AM40-AM41</f>
-        <v>4923.1160468037906</v>
+        <v>4906.3886987639034</v>
       </c>
       <c r="AN42" s="4">
         <f t="shared" ref="AN42:AU42" si="86">+AN40-AN41</f>
-        <v>5339.3519394324139</v>
+        <v>5317.8916605189579</v>
       </c>
       <c r="AO42" s="4">
         <f t="shared" si="86"/>
-        <v>5769.4898846589786</v>
+        <v>5743.1504343087008</v>
       </c>
       <c r="AP42" s="4">
         <f t="shared" si="86"/>
-        <v>6213.9428143310024</v>
+        <v>6182.5754509597718</v>
       </c>
       <c r="AQ42" s="4">
         <f t="shared" si="86"/>
-        <v>6673.1339164258625</v>
+        <v>6636.5874141012237</v>
       </c>
       <c r="AR42" s="4">
         <f t="shared" si="86"/>
-        <v>7147.4969011328949</v>
+        <v>7105.6175702426344</v>
       </c>
       <c r="AS42" s="4">
         <f t="shared" si="86"/>
-        <v>7637.4762728461292</v>
+        <v>7590.1079850091519</v>
       </c>
       <c r="AT42" s="4">
         <f t="shared" si="86"/>
-        <v>8143.5276082164055</v>
+        <v>8090.5118256942187</v>
       </c>
       <c r="AU42" s="4">
         <f t="shared" si="86"/>
-        <v>8666.1178404148432</v>
+        <v>8607.2936502944758</v>
       </c>
       <c r="AV42" s="4">
         <f t="shared" ref="AV42" si="87">+AV40-AV41</f>
-        <v>9205.7255497627448</v>
+        <v>9140.9297031949536</v>
       </c>
     </row>
     <row r="43" spans="2:246">
@@ -6056,835 +6066,835 @@
       </c>
       <c r="AM44" s="6">
         <f>+AM42-AM43</f>
-        <v>4923.1160468037906</v>
+        <v>4906.3886987639034</v>
       </c>
       <c r="AN44" s="6">
         <f t="shared" ref="AN44:AU44" si="95">+AN42-AN43</f>
-        <v>5339.3519394324139</v>
+        <v>5317.8916605189579</v>
       </c>
       <c r="AO44" s="6">
         <f t="shared" si="95"/>
-        <v>5769.4898846589786</v>
+        <v>5743.1504343087008</v>
       </c>
       <c r="AP44" s="6">
         <f t="shared" si="95"/>
-        <v>6213.9428143310024</v>
+        <v>6182.5754509597718</v>
       </c>
       <c r="AQ44" s="6">
         <f t="shared" si="95"/>
-        <v>6673.1339164258625</v>
+        <v>6636.5874141012237</v>
       </c>
       <c r="AR44" s="6">
         <f t="shared" si="95"/>
-        <v>7147.4969011328949</v>
+        <v>7105.6175702426344</v>
       </c>
       <c r="AS44" s="6">
         <f t="shared" si="95"/>
-        <v>7637.4762728461292</v>
+        <v>7590.1079850091519</v>
       </c>
       <c r="AT44" s="6">
         <f t="shared" si="95"/>
-        <v>8143.5276082164055</v>
+        <v>8090.5118256942187</v>
       </c>
       <c r="AU44" s="6">
         <f t="shared" si="95"/>
-        <v>8666.1178404148432</v>
+        <v>8607.2936502944758</v>
       </c>
       <c r="AV44" s="6">
         <f t="shared" ref="AV44" si="96">+AV42-AV43</f>
-        <v>9205.7255497627448</v>
+        <v>9140.9297031949536</v>
       </c>
       <c r="AW44" s="6">
         <f t="shared" ref="AW44:CB44" si="97">+AV44*(1+$AY$49)</f>
-        <v>9389.8400607580006</v>
+        <v>9323.7482972588532</v>
       </c>
       <c r="AX44" s="6">
         <f t="shared" si="97"/>
-        <v>9577.6368619731602</v>
+        <v>9510.2232632040304</v>
       </c>
       <c r="AY44" s="6">
         <f t="shared" si="97"/>
-        <v>9769.1895992126229</v>
+        <v>9700.427728468112</v>
       </c>
       <c r="AZ44" s="6">
         <f t="shared" si="97"/>
-        <v>9964.5733911968746</v>
+        <v>9894.4362830374739</v>
       </c>
       <c r="BA44" s="6">
         <f t="shared" si="97"/>
-        <v>10163.864859020812</v>
+        <v>10092.325008698224</v>
       </c>
       <c r="BB44" s="6">
         <f t="shared" si="97"/>
-        <v>10367.142156201229</v>
+        <v>10294.171508872188</v>
       </c>
       <c r="BC44" s="6">
         <f t="shared" si="97"/>
-        <v>10574.484999325254</v>
+        <v>10500.054939049633</v>
       </c>
       <c r="BD44" s="6">
         <f t="shared" si="97"/>
-        <v>10785.974699311759</v>
+        <v>10710.056037830625</v>
       </c>
       <c r="BE44" s="6">
         <f t="shared" si="97"/>
-        <v>11001.694193297993</v>
+        <v>10924.257158587237</v>
       </c>
       <c r="BF44" s="6">
         <f t="shared" si="97"/>
-        <v>11221.728077163954</v>
+        <v>11142.742301758983</v>
       </c>
       <c r="BG44" s="6">
         <f t="shared" si="97"/>
-        <v>11446.162638707234</v>
+        <v>11365.597147794162</v>
       </c>
       <c r="BH44" s="6">
         <f t="shared" si="97"/>
-        <v>11675.085891481378</v>
+        <v>11592.909090750045</v>
       </c>
       <c r="BI44" s="6">
         <f t="shared" si="97"/>
-        <v>11908.587609311006</v>
+        <v>11824.767272565046</v>
       </c>
       <c r="BJ44" s="6">
         <f t="shared" si="97"/>
-        <v>12146.759361497227</v>
+        <v>12061.262618016348</v>
       </c>
       <c r="BK44" s="6">
         <f t="shared" si="97"/>
-        <v>12389.694548727171</v>
+        <v>12302.487870376675</v>
       </c>
       <c r="BL44" s="6">
         <f t="shared" si="97"/>
-        <v>12637.488439701716</v>
+        <v>12548.53762778421</v>
       </c>
       <c r="BM44" s="6">
         <f t="shared" si="97"/>
-        <v>12890.23820849575</v>
+        <v>12799.508380339894</v>
       </c>
       <c r="BN44" s="6">
         <f t="shared" si="97"/>
-        <v>13148.042972665666</v>
+        <v>13055.498547946692</v>
       </c>
       <c r="BO44" s="6">
         <f t="shared" si="97"/>
-        <v>13411.003832118979</v>
+        <v>13316.608518905627</v>
       </c>
       <c r="BP44" s="6">
         <f t="shared" si="97"/>
-        <v>13679.223908761358</v>
+        <v>13582.94068928374</v>
       </c>
       <c r="BQ44" s="6">
         <f t="shared" si="97"/>
-        <v>13952.808386936586</v>
+        <v>13854.599503069414</v>
       </c>
       <c r="BR44" s="6">
         <f t="shared" si="97"/>
-        <v>14231.864554675318</v>
+        <v>14131.691493130802</v>
       </c>
       <c r="BS44" s="6">
         <f t="shared" si="97"/>
-        <v>14516.501845768824</v>
+        <v>14414.325322993418</v>
       </c>
       <c r="BT44" s="6">
         <f t="shared" si="97"/>
-        <v>14806.831882684201</v>
+        <v>14702.611829453286</v>
       </c>
       <c r="BU44" s="6">
         <f t="shared" si="97"/>
-        <v>15102.968520337885</v>
+        <v>14996.664066042353</v>
       </c>
       <c r="BV44" s="6">
         <f t="shared" si="97"/>
-        <v>15405.027890744643</v>
+        <v>15296.5973473632</v>
       </c>
       <c r="BW44" s="6">
         <f t="shared" si="97"/>
-        <v>15713.128448559535</v>
+        <v>15602.529294310465</v>
       </c>
       <c r="BX44" s="6">
         <f t="shared" si="97"/>
-        <v>16027.391017530726</v>
+        <v>15914.579880196674</v>
       </c>
       <c r="BY44" s="6">
         <f t="shared" si="97"/>
-        <v>16347.938837881342</v>
+        <v>16232.871477800607</v>
       </c>
       <c r="BZ44" s="6">
         <f t="shared" si="97"/>
-        <v>16674.897614638969</v>
+        <v>16557.52890735662</v>
       </c>
       <c r="CA44" s="6">
         <f t="shared" si="97"/>
-        <v>17008.395566931747</v>
+        <v>16888.679485503751</v>
       </c>
       <c r="CB44" s="6">
         <f t="shared" si="97"/>
-        <v>17348.563478270382</v>
+        <v>17226.453075213827</v>
       </c>
       <c r="CC44" s="6">
         <f t="shared" ref="CC44:DH44" si="98">+CB44*(1+$AY$49)</f>
-        <v>17695.534747835791</v>
+        <v>17570.982136718103</v>
       </c>
       <c r="CD44" s="6">
         <f t="shared" si="98"/>
-        <v>18049.445442792508</v>
+        <v>17922.401779452466</v>
       </c>
       <c r="CE44" s="6">
         <f t="shared" si="98"/>
-        <v>18410.43435164836</v>
+        <v>18280.849815041514</v>
       </c>
       <c r="CF44" s="6">
         <f t="shared" si="98"/>
-        <v>18778.643038681326</v>
+        <v>18646.466811342347</v>
       </c>
       <c r="CG44" s="6">
         <f t="shared" si="98"/>
-        <v>19154.215899454954</v>
+        <v>19019.396147569194</v>
       </c>
       <c r="CH44" s="6">
         <f t="shared" si="98"/>
-        <v>19537.300217444052</v>
+        <v>19399.784070520578</v>
       </c>
       <c r="CI44" s="6">
         <f t="shared" si="98"/>
-        <v>19928.046221792934</v>
+        <v>19787.77975193099</v>
       </c>
       <c r="CJ44" s="6">
         <f t="shared" si="98"/>
-        <v>20326.607146228795</v>
+        <v>20183.535346969609</v>
       </c>
       <c r="CK44" s="6">
         <f t="shared" si="98"/>
-        <v>20733.139289153372</v>
+        <v>20587.206053909002</v>
       </c>
       <c r="CL44" s="6">
         <f t="shared" si="98"/>
-        <v>21147.80207493644</v>
+        <v>20998.950174987182</v>
       </c>
       <c r="CM44" s="6">
         <f t="shared" si="98"/>
-        <v>21570.758116435169</v>
+        <v>21418.929178486924</v>
       </c>
       <c r="CN44" s="6">
         <f t="shared" si="98"/>
-        <v>22002.173278763872</v>
+        <v>21847.307762056662</v>
       </c>
       <c r="CO44" s="6">
         <f t="shared" si="98"/>
-        <v>22442.216744339148</v>
+        <v>22284.253917297796</v>
       </c>
       <c r="CP44" s="6">
         <f t="shared" si="98"/>
-        <v>22891.061079225932</v>
+        <v>22729.938995643752</v>
       </c>
       <c r="CQ44" s="6">
         <f t="shared" si="98"/>
-        <v>23348.882300810452</v>
+        <v>23184.537775556626</v>
       </c>
       <c r="CR44" s="6">
         <f t="shared" si="98"/>
-        <v>23815.859946826662</v>
+        <v>23648.228531067758</v>
       </c>
       <c r="CS44" s="6">
         <f t="shared" si="98"/>
-        <v>24292.177145763195</v>
+        <v>24121.193101689114</v>
       </c>
       <c r="CT44" s="6">
         <f t="shared" si="98"/>
-        <v>24778.020688678458</v>
+        <v>24603.616963722896</v>
       </c>
       <c r="CU44" s="6">
         <f t="shared" si="98"/>
-        <v>25273.581102452026</v>
+        <v>25095.689302997354</v>
       </c>
       <c r="CV44" s="6">
         <f t="shared" si="98"/>
-        <v>25779.052724501067</v>
+        <v>25597.603089057302</v>
       </c>
       <c r="CW44" s="6">
         <f t="shared" si="98"/>
-        <v>26294.63377899109</v>
+        <v>26109.555150838449</v>
       </c>
       <c r="CX44" s="6">
         <f t="shared" si="98"/>
-        <v>26820.526454570914</v>
+        <v>26631.746253855217</v>
       </c>
       <c r="CY44" s="6">
         <f t="shared" si="98"/>
-        <v>27356.936983662334</v>
+        <v>27164.381178932323</v>
       </c>
       <c r="CZ44" s="6">
         <f t="shared" si="98"/>
-        <v>27904.07572333558</v>
+        <v>27707.668802510969</v>
       </c>
       <c r="DA44" s="6">
         <f t="shared" si="98"/>
-        <v>28462.15723780229</v>
+        <v>28261.82217856119</v>
       </c>
       <c r="DB44" s="6">
         <f t="shared" si="98"/>
-        <v>29031.400382558335</v>
+        <v>28827.058622132412</v>
       </c>
       <c r="DC44" s="6">
         <f t="shared" si="98"/>
-        <v>29612.028390209503</v>
+        <v>29403.599794575061</v>
       </c>
       <c r="DD44" s="6">
         <f t="shared" si="98"/>
-        <v>30204.268958013694</v>
+        <v>29991.671790466564</v>
       </c>
       <c r="DE44" s="6">
         <f t="shared" si="98"/>
-        <v>30808.354337173969</v>
+        <v>30591.505226275895</v>
       </c>
       <c r="DF44" s="6">
         <f t="shared" si="98"/>
-        <v>31424.521423917449</v>
+        <v>31203.335330801412</v>
       </c>
       <c r="DG44" s="6">
         <f t="shared" si="98"/>
-        <v>32053.011852395797</v>
+        <v>31827.40203741744</v>
       </c>
       <c r="DH44" s="6">
         <f t="shared" si="98"/>
-        <v>32694.072089443715</v>
+        <v>32463.950078165788</v>
       </c>
       <c r="DI44" s="6">
         <f t="shared" ref="DI44:EN44" si="99">+DH44*(1+$AY$49)</f>
-        <v>33347.95353123259</v>
+        <v>33113.229079729106</v>
       </c>
       <c r="DJ44" s="6">
         <f t="shared" si="99"/>
-        <v>34014.912601857242</v>
+        <v>33775.493661323686</v>
       </c>
       <c r="DK44" s="6">
         <f t="shared" si="99"/>
-        <v>34695.210853894387</v>
+        <v>34451.00353455016</v>
       </c>
       <c r="DL44" s="6">
         <f t="shared" si="99"/>
-        <v>35389.115070972271</v>
+        <v>35140.023605241164</v>
       </c>
       <c r="DM44" s="6">
         <f t="shared" si="99"/>
-        <v>36096.897372391715</v>
+        <v>35842.824077345991</v>
       </c>
       <c r="DN44" s="6">
         <f t="shared" si="99"/>
-        <v>36818.835319839549</v>
+        <v>36559.680558892913</v>
       </c>
       <c r="DO44" s="6">
         <f t="shared" si="99"/>
-        <v>37555.212026236339</v>
+        <v>37290.874170070769</v>
       </c>
       <c r="DP44" s="6">
         <f t="shared" si="99"/>
-        <v>38306.316266761067</v>
+        <v>38036.691653472182</v>
       </c>
       <c r="DQ44" s="6">
         <f t="shared" si="99"/>
-        <v>39072.442592096289</v>
+        <v>38797.42548654163</v>
       </c>
       <c r="DR44" s="6">
         <f t="shared" si="99"/>
-        <v>39853.891443938213</v>
+        <v>39573.373996272465</v>
       </c>
       <c r="DS44" s="6">
         <f t="shared" si="99"/>
-        <v>40650.969272816976</v>
+        <v>40364.841476197915</v>
       </c>
       <c r="DT44" s="6">
         <f t="shared" si="99"/>
-        <v>41463.988658273316</v>
+        <v>41172.138305721877</v>
       </c>
       <c r="DU44" s="6">
         <f t="shared" si="99"/>
-        <v>42293.268431438781</v>
+        <v>41995.581071836314</v>
       </c>
       <c r="DV44" s="6">
         <f t="shared" si="99"/>
-        <v>43139.133800067561</v>
+        <v>42835.492693273038</v>
       </c>
       <c r="DW44" s="6">
         <f t="shared" si="99"/>
-        <v>44001.916476068909</v>
+        <v>43692.202547138499</v>
       </c>
       <c r="DX44" s="6">
         <f t="shared" si="99"/>
-        <v>44881.954805590285</v>
+        <v>44566.046598081266</v>
       </c>
       <c r="DY44" s="6">
         <f t="shared" si="99"/>
-        <v>45779.593901702094</v>
+        <v>45457.367530042895</v>
       </c>
       <c r="DZ44" s="6">
         <f t="shared" si="99"/>
-        <v>46695.185779736137</v>
+        <v>46366.51488064375</v>
       </c>
       <c r="EA44" s="6">
         <f t="shared" si="99"/>
-        <v>47629.08949533086</v>
+        <v>47293.845178256626</v>
       </c>
       <c r="EB44" s="6">
         <f t="shared" si="99"/>
-        <v>48581.671285237477</v>
+        <v>48239.722081821761</v>
       </c>
       <c r="EC44" s="6">
         <f t="shared" si="99"/>
-        <v>49553.304710942226</v>
+        <v>49204.516523458195</v>
       </c>
       <c r="ED44" s="6">
         <f t="shared" si="99"/>
-        <v>50544.370805161074</v>
+        <v>50188.606853927362</v>
       </c>
       <c r="EE44" s="6">
         <f t="shared" si="99"/>
-        <v>51555.258221264296</v>
+        <v>51192.378991005913</v>
       </c>
       <c r="EF44" s="6">
         <f t="shared" si="99"/>
-        <v>52586.363385689583</v>
+        <v>52216.226570826031</v>
       </c>
       <c r="EG44" s="6">
         <f t="shared" si="99"/>
-        <v>53638.090653403378</v>
+        <v>53260.551102242556</v>
       </c>
       <c r="EH44" s="6">
         <f t="shared" si="99"/>
-        <v>54710.85246647145</v>
+        <v>54325.762124287408</v>
       </c>
       <c r="EI44" s="6">
         <f t="shared" si="99"/>
-        <v>55805.069515800882</v>
+        <v>55412.27736677316</v>
       </c>
       <c r="EJ44" s="6">
         <f t="shared" si="99"/>
-        <v>56921.170906116902</v>
+        <v>56520.522914108624</v>
       </c>
       <c r="EK44" s="6">
         <f t="shared" si="99"/>
-        <v>58059.594324239239</v>
+        <v>57650.933372390798</v>
       </c>
       <c r="EL44" s="6">
         <f t="shared" si="99"/>
-        <v>59220.786210724022</v>
+        <v>58803.952039838616</v>
       </c>
       <c r="EM44" s="6">
         <f t="shared" si="99"/>
-        <v>60405.201934938501</v>
+        <v>59980.031080635388</v>
       </c>
       <c r="EN44" s="6">
         <f t="shared" si="99"/>
-        <v>61613.305973637274</v>
+        <v>61179.631702248094</v>
       </c>
       <c r="EO44" s="6">
         <f t="shared" ref="EO44:FT44" si="100">+EN44*(1+$AY$49)</f>
-        <v>62845.572093110022</v>
+        <v>62403.22433629306</v>
       </c>
       <c r="EP44" s="6">
         <f t="shared" si="100"/>
-        <v>64102.483534972227</v>
+        <v>63651.28882301892</v>
       </c>
       <c r="EQ44" s="6">
         <f t="shared" si="100"/>
-        <v>65384.533205671672</v>
+        <v>64924.314599479301</v>
       </c>
       <c r="ER44" s="6">
         <f t="shared" si="100"/>
-        <v>66692.223869785113</v>
+        <v>66222.800891468883</v>
       </c>
       <c r="ES44" s="6">
         <f t="shared" si="100"/>
-        <v>68026.068347180815</v>
+        <v>67547.256909298259</v>
       </c>
       <c r="ET44" s="6">
         <f t="shared" si="100"/>
-        <v>69386.589714124435</v>
+        <v>68898.202047484228</v>
       </c>
       <c r="EU44" s="6">
         <f t="shared" si="100"/>
-        <v>70774.321508406923</v>
+        <v>70276.166088433907</v>
       </c>
       <c r="EV44" s="6">
         <f t="shared" si="100"/>
-        <v>72189.807938575061</v>
+        <v>71681.689410202584</v>
       </c>
       <c r="EW44" s="6">
         <f t="shared" si="100"/>
-        <v>73633.604097346557</v>
+        <v>73115.323198406637</v>
       </c>
       <c r="EX44" s="6">
         <f t="shared" si="100"/>
-        <v>75106.276179293491</v>
+        <v>74577.629662374777</v>
       </c>
       <c r="EY44" s="6">
         <f t="shared" si="100"/>
-        <v>76608.401702879361</v>
+        <v>76069.182255622276</v>
       </c>
       <c r="EZ44" s="6">
         <f t="shared" si="100"/>
-        <v>78140.569736936945</v>
+        <v>77590.565900734728</v>
       </c>
       <c r="FA44" s="6">
         <f t="shared" si="100"/>
-        <v>79703.381131675691</v>
+        <v>79142.377218749418</v>
       </c>
       <c r="FB44" s="6">
         <f t="shared" si="100"/>
-        <v>81297.448754309211</v>
+        <v>80725.22476312441</v>
       </c>
       <c r="FC44" s="6">
         <f t="shared" si="100"/>
-        <v>82923.397729395394</v>
+        <v>82339.729258386898</v>
       </c>
       <c r="FD44" s="6">
         <f t="shared" si="100"/>
-        <v>84581.865683983298</v>
+        <v>83986.523843554634</v>
       </c>
       <c r="FE44" s="6">
         <f t="shared" si="100"/>
-        <v>86273.502997662959</v>
+        <v>85666.254320425724</v>
       </c>
       <c r="FF44" s="6">
         <f t="shared" si="100"/>
-        <v>87998.973057616226</v>
+        <v>87379.579406834237</v>
       </c>
       <c r="FG44" s="6">
         <f t="shared" si="100"/>
-        <v>89758.95251876855</v>
+        <v>89127.170994970918</v>
       </c>
       <c r="FH44" s="6">
         <f t="shared" si="100"/>
-        <v>91554.131569143923</v>
+        <v>90909.714414870337</v>
       </c>
       <c r="FI44" s="6">
         <f t="shared" si="100"/>
-        <v>93385.214200526796</v>
+        <v>92727.908703167748</v>
       </c>
       <c r="FJ44" s="6">
         <f t="shared" si="100"/>
-        <v>95252.918484537338</v>
+        <v>94582.466877231098</v>
       </c>
       <c r="FK44" s="6">
         <f t="shared" si="100"/>
-        <v>97157.97685422808</v>
+        <v>96474.116214775728</v>
       </c>
       <c r="FL44" s="6">
         <f t="shared" si="100"/>
-        <v>99101.136391312641</v>
+        <v>98403.598539071245</v>
       </c>
       <c r="FM44" s="6">
         <f t="shared" si="100"/>
-        <v>101083.1591191389</v>
+        <v>100371.67050985267</v>
       </c>
       <c r="FN44" s="6">
         <f t="shared" si="100"/>
-        <v>103104.82230152168</v>
+        <v>102379.10392004973</v>
       </c>
       <c r="FO44" s="6">
         <f t="shared" si="100"/>
-        <v>105166.91874755212</v>
+        <v>104426.68599845073</v>
       </c>
       <c r="FP44" s="6">
         <f t="shared" si="100"/>
-        <v>107270.25712250316</v>
+        <v>106515.21971841974</v>
       </c>
       <c r="FQ44" s="6">
         <f t="shared" si="100"/>
-        <v>109415.66226495322</v>
+        <v>108645.52411278815</v>
       </c>
       <c r="FR44" s="6">
         <f t="shared" si="100"/>
-        <v>111603.97551025229</v>
+        <v>110818.43459504392</v>
       </c>
       <c r="FS44" s="6">
         <f t="shared" si="100"/>
-        <v>113836.05502045734</v>
+        <v>113034.80328694479</v>
       </c>
       <c r="FT44" s="6">
         <f t="shared" si="100"/>
-        <v>116112.77612086649</v>
+        <v>115295.49935268369</v>
       </c>
       <c r="FU44" s="6">
         <f t="shared" ref="FU44:GZ44" si="101">+FT44*(1+$AY$49)</f>
-        <v>118435.03164328382</v>
+        <v>117601.40933973737</v>
       </c>
       <c r="FV44" s="6">
         <f t="shared" si="101"/>
-        <v>120803.73227614949</v>
+        <v>119953.43752653211</v>
       </c>
       <c r="FW44" s="6">
         <f t="shared" si="101"/>
-        <v>123219.80692167248</v>
+        <v>122352.50627706276</v>
       </c>
       <c r="FX44" s="6">
         <f t="shared" si="101"/>
-        <v>125684.20306010594</v>
+        <v>124799.55640260401</v>
       </c>
       <c r="FY44" s="6">
         <f t="shared" si="101"/>
-        <v>128197.88712130806</v>
+        <v>127295.54753065608</v>
       </c>
       <c r="FZ44" s="6">
         <f t="shared" si="101"/>
-        <v>130761.84486373422</v>
+        <v>129841.4584812692</v>
       </c>
       <c r="GA44" s="6">
         <f t="shared" si="101"/>
-        <v>133377.08176100891</v>
+        <v>132438.28765089458</v>
       </c>
       <c r="GB44" s="6">
         <f t="shared" si="101"/>
-        <v>136044.62339622909</v>
+        <v>135087.05340391246</v>
       </c>
       <c r="GC44" s="6">
         <f t="shared" si="101"/>
-        <v>138765.51586415368</v>
+        <v>137788.79447199072</v>
       </c>
       <c r="GD44" s="6">
         <f t="shared" si="101"/>
-        <v>141540.82618143677</v>
+        <v>140544.57036143055</v>
       </c>
       <c r="GE44" s="6">
         <f t="shared" si="101"/>
-        <v>144371.64270506552</v>
+        <v>143355.46176865918</v>
       </c>
       <c r="GF44" s="6">
         <f t="shared" si="101"/>
-        <v>147259.07555916684</v>
+        <v>146222.57100403236</v>
       </c>
       <c r="GG44" s="6">
         <f t="shared" si="101"/>
-        <v>150204.25707035017</v>
+        <v>149147.02242411301</v>
       </c>
       <c r="GH44" s="6">
         <f t="shared" si="101"/>
-        <v>153208.34221175718</v>
+        <v>152129.96287259526</v>
       </c>
       <c r="GI44" s="6">
         <f t="shared" si="101"/>
-        <v>156272.50905599233</v>
+        <v>155172.56213004718</v>
       </c>
       <c r="GJ44" s="6">
         <f t="shared" si="101"/>
-        <v>159397.95923711217</v>
+        <v>158276.01337264813</v>
       </c>
       <c r="GK44" s="6">
         <f t="shared" si="101"/>
-        <v>162585.91842185441</v>
+        <v>161441.53364010109</v>
       </c>
       <c r="GL44" s="6">
         <f t="shared" si="101"/>
-        <v>165837.63679029149</v>
+        <v>164670.36431290311</v>
       </c>
       <c r="GM44" s="6">
         <f t="shared" si="101"/>
-        <v>169154.38952609734</v>
+        <v>167963.77159916118</v>
       </c>
       <c r="GN44" s="6">
         <f t="shared" si="101"/>
-        <v>172537.47731661928</v>
+        <v>171323.04703114441</v>
       </c>
       <c r="GO44" s="6">
         <f t="shared" si="101"/>
-        <v>175988.22686295168</v>
+        <v>174749.50797176731</v>
       </c>
       <c r="GP44" s="6">
         <f t="shared" si="101"/>
-        <v>179507.99140021071</v>
+        <v>178244.49813120265</v>
       </c>
       <c r="GQ44" s="6">
         <f t="shared" si="101"/>
-        <v>183098.15122821493</v>
+        <v>181809.38809382671</v>
       </c>
       <c r="GR44" s="6">
         <f t="shared" si="101"/>
-        <v>186760.11425277923</v>
+        <v>185445.57585570324</v>
       </c>
       <c r="GS44" s="6">
         <f t="shared" si="101"/>
-        <v>190495.31653783482</v>
+        <v>189154.4873728173</v>
       </c>
       <c r="GT44" s="6">
         <f t="shared" si="101"/>
-        <v>194305.22286859152</v>
+        <v>192937.57712027364</v>
       </c>
       <c r="GU44" s="6">
         <f t="shared" si="101"/>
-        <v>198191.32732596336</v>
+        <v>196796.32866267912</v>
       </c>
       <c r="GV44" s="6">
         <f t="shared" si="101"/>
-        <v>202155.15387248262</v>
+        <v>200732.25523593271</v>
       </c>
       <c r="GW44" s="6">
         <f t="shared" si="101"/>
-        <v>206198.25694993229</v>
+        <v>204746.90034065137</v>
       </c>
       <c r="GX44" s="6">
         <f t="shared" si="101"/>
-        <v>210322.22208893092</v>
+        <v>208841.83834746439</v>
       </c>
       <c r="GY44" s="6">
         <f t="shared" si="101"/>
-        <v>214528.66653070954</v>
+        <v>213018.67511441369</v>
       </c>
       <c r="GZ44" s="6">
         <f t="shared" si="101"/>
-        <v>218819.23986132373</v>
+        <v>217279.04861670197</v>
       </c>
       <c r="HA44" s="6">
         <f t="shared" ref="HA44:IF44" si="102">+GZ44*(1+$AY$49)</f>
-        <v>223195.62465855022</v>
+        <v>221624.62958903602</v>
       </c>
       <c r="HB44" s="6">
         <f t="shared" si="102"/>
-        <v>227659.53715172122</v>
+        <v>226057.12218081675</v>
       </c>
       <c r="HC44" s="6">
         <f t="shared" si="102"/>
-        <v>232212.72789475563</v>
+        <v>230578.2646244331</v>
       </c>
       <c r="HD44" s="6">
         <f t="shared" si="102"/>
-        <v>236856.98245265076</v>
+        <v>235189.82991692176</v>
       </c>
       <c r="HE44" s="6">
         <f t="shared" si="102"/>
-        <v>241594.12210170378</v>
+        <v>239893.6265152602</v>
       </c>
       <c r="HF44" s="6">
         <f t="shared" si="102"/>
-        <v>246426.00454373786</v>
+        <v>244691.4990455654</v>
       </c>
       <c r="HG44" s="6">
         <f t="shared" si="102"/>
-        <v>251354.52463461261</v>
+        <v>249585.32902647671</v>
       </c>
       <c r="HH44" s="6">
         <f t="shared" si="102"/>
-        <v>256381.61512730486</v>
+        <v>254577.03560700626</v>
       </c>
       <c r="HI44" s="6">
         <f t="shared" si="102"/>
-        <v>261509.24742985095</v>
+        <v>259668.57631914638</v>
       </c>
       <c r="HJ44" s="6">
         <f t="shared" si="102"/>
-        <v>266739.43237844796</v>
+        <v>264861.9478455293</v>
       </c>
       <c r="HK44" s="6">
         <f t="shared" si="102"/>
-        <v>272074.22102601692</v>
+        <v>270159.18680243992</v>
       </c>
       <c r="HL44" s="6">
         <f t="shared" si="102"/>
-        <v>277515.70544653729</v>
+        <v>275562.37053848873</v>
       </c>
       <c r="HM44" s="6">
         <f t="shared" si="102"/>
-        <v>283066.01955546805</v>
+        <v>281073.61794925854</v>
       </c>
       <c r="HN44" s="6">
         <f t="shared" si="102"/>
-        <v>288727.33994657744</v>
+        <v>286695.0903082437</v>
       </c>
       <c r="HO44" s="6">
         <f t="shared" si="102"/>
-        <v>294501.88674550899</v>
+        <v>292428.99211440858</v>
       </c>
       <c r="HP44" s="6">
         <f t="shared" si="102"/>
-        <v>300391.9244804192</v>
+        <v>298277.57195669675</v>
       </c>
       <c r="HQ44" s="6">
         <f t="shared" si="102"/>
-        <v>306399.76297002757</v>
+        <v>304243.12339583068</v>
       </c>
       <c r="HR44" s="6">
         <f t="shared" si="102"/>
-        <v>312527.75822942815</v>
+        <v>310327.98586374731</v>
       </c>
       <c r="HS44" s="6">
         <f t="shared" si="102"/>
-        <v>318778.3133940167</v>
+        <v>316534.54558102228</v>
       </c>
       <c r="HT44" s="6">
         <f t="shared" si="102"/>
-        <v>325153.87966189702</v>
+        <v>322865.23649264273</v>
       </c>
       <c r="HU44" s="6">
         <f t="shared" si="102"/>
-        <v>331656.95725513494</v>
+        <v>329322.54122249561</v>
       </c>
       <c r="HV44" s="6">
         <f t="shared" si="102"/>
-        <v>338290.09640023764</v>
+        <v>335908.99204694555</v>
       </c>
       <c r="HW44" s="6">
         <f t="shared" si="102"/>
-        <v>345055.89832824242</v>
+        <v>342627.1718878845</v>
       </c>
       <c r="HX44" s="6">
         <f t="shared" si="102"/>
-        <v>351957.01629480725</v>
+        <v>349479.7153256422</v>
       </c>
       <c r="HY44" s="6">
         <f t="shared" si="102"/>
-        <v>358996.1566207034</v>
+        <v>356469.30963215505</v>
       </c>
       <c r="HZ44" s="6">
         <f t="shared" si="102"/>
-        <v>366176.07975311746</v>
+        <v>363598.69582479814</v>
       </c>
       <c r="IA44" s="6">
         <f t="shared" si="102"/>
-        <v>373499.6013481798</v>
+        <v>370870.66974129411</v>
       </c>
       <c r="IB44" s="6">
         <f t="shared" si="102"/>
-        <v>380969.59337514342</v>
+        <v>378288.08313612</v>
       </c>
       <c r="IC44" s="6">
         <f t="shared" si="102"/>
-        <v>388588.9852426463</v>
+        <v>385853.84479884239</v>
       </c>
       <c r="ID44" s="6">
         <f t="shared" si="102"/>
-        <v>396360.76494749926</v>
+        <v>393570.92169481923</v>
       </c>
       <c r="IE44" s="6">
         <f t="shared" si="102"/>
-        <v>404287.98024644924</v>
+        <v>401442.34012871562</v>
       </c>
       <c r="IF44" s="6">
         <f t="shared" si="102"/>
-        <v>412373.73985137825</v>
+        <v>409471.18693128991</v>
       </c>
       <c r="IG44" s="6">
         <f t="shared" ref="IG44:IL44" si="103">+IF44*(1+$AY$49)</f>
-        <v>420621.21464840585</v>
+        <v>417660.61066991574</v>
       </c>
       <c r="IH44" s="6">
         <f t="shared" si="103"/>
-        <v>429033.63894137397</v>
+        <v>426013.82288331405</v>
       </c>
       <c r="II44" s="6">
         <f t="shared" si="103"/>
-        <v>437614.31172020145</v>
+        <v>434534.09934098035</v>
       </c>
       <c r="IJ44" s="6">
         <f t="shared" si="103"/>
-        <v>446366.59795460547</v>
+        <v>443224.78132779995</v>
       </c>
       <c r="IK44" s="6">
         <f t="shared" si="103"/>
-        <v>455293.92991369759</v>
+        <v>452089.27695435594</v>
       </c>
       <c r="IL44" s="6">
         <f t="shared" si="103"/>
-        <v>464399.80851197155</v>
+        <v>461131.06249344308</v>
       </c>
     </row>
     <row r="45" spans="2:246">
@@ -7152,43 +7162,43 @@
       </c>
       <c r="AM46" s="3">
         <f>+AM44/AM45</f>
-        <v>3.9708808017529575</v>
+        <v>3.957388878230466</v>
       </c>
       <c r="AN46" s="3">
         <f t="shared" ref="AN46:AU46" si="113">+AN44/AN45</f>
-        <v>4.3066078289703151</v>
+        <v>4.2892984239659313</v>
       </c>
       <c r="AO46" s="3">
         <f t="shared" si="113"/>
-        <v>4.6535479564358306</v>
+        <v>4.6323031154184129</v>
       </c>
       <c r="AP46" s="3">
         <f t="shared" si="113"/>
-        <v>5.0120342462041352</v>
+        <v>4.9867339973722409</v>
       </c>
       <c r="AQ46" s="3">
         <f t="shared" si="113"/>
-        <v>5.3824080327062953</v>
+        <v>5.3529304004359073</v>
       </c>
       <c r="AR46" s="3">
         <f t="shared" si="113"/>
-        <v>5.7650191373659734</v>
+        <v>5.7312401588813282</v>
       </c>
       <c r="AS46" s="3">
         <f t="shared" si="113"/>
-        <v>6.1602260879829958</v>
+        <v>6.1220198334491673</v>
       </c>
       <c r="AT46" s="3">
         <f t="shared" si="113"/>
-        <v>6.56839634300428</v>
+        <v>6.5256349392498558</v>
       </c>
       <c r="AU46" s="3">
         <f t="shared" si="113"/>
-        <v>6.9899065208047055</v>
+        <v>6.9424601788930049</v>
       </c>
       <c r="AV46" s="3">
         <f t="shared" ref="AV46" si="114">+AV44/AV45</f>
-        <v>7.4251426341030262</v>
+        <v>7.3728796809808026</v>
       </c>
     </row>
     <row r="47" spans="2:246">
@@ -7196,7 +7206,7 @@
         <v>149</v>
       </c>
       <c r="AY47" s="30">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="48" spans="2:246">
@@ -7355,10 +7365,10 @@
         <f t="shared" si="125"/>
         <v>5.9740259740259871E-2</v>
       </c>
-      <c r="AX49" s="33" t="s">
+      <c r="AX49" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="AY49" s="34">
+      <c r="AY49" s="32">
         <v>0.02</v>
       </c>
     </row>
@@ -7502,7 +7512,7 @@
         <f t="shared" ref="AV50" si="129">+AV34/AV24</f>
         <v>0.18950521390498698</v>
       </c>
-      <c r="AX50" s="33" t="s">
+      <c r="AX50" s="36" t="s">
         <v>45</v>
       </c>
       <c r="AY50" s="32">
@@ -7514,16 +7524,16 @@
       <c r="AX51" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="AY51" s="35">
+      <c r="AY51" s="33">
         <f>NPV(AY50,AL44:IL44)</f>
-        <v>111624.14377226394</v>
+        <v>110925.02099759961</v>
       </c>
     </row>
     <row r="52" spans="2:51">
       <c r="AX52" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="AY52" s="35">
+      <c r="AY52" s="33">
         <f>+V57</f>
         <v>-11581.9</v>
       </c>
@@ -7532,36 +7542,36 @@
       <c r="AX53" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="AY53" s="35">
+      <c r="AY53" s="33">
         <f>+AY51+AY52</f>
-        <v>100042.24377226394</v>
+        <v>99343.120997599617</v>
       </c>
     </row>
     <row r="54" spans="2:51">
       <c r="AX54" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="AY54" s="35">
+      <c r="AY54" s="33">
         <f>+Main!I8</f>
         <v>1158.5</v>
       </c>
     </row>
     <row r="55" spans="2:51">
-      <c r="AX55" s="31" t="s">
+      <c r="AX55" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="AY55" s="35">
+      <c r="AY55" s="38">
         <f>+AY53/AY54</f>
-        <v>86.354979518570516</v>
+        <v>85.751507119205542</v>
       </c>
     </row>
     <row r="56" spans="2:51">
       <c r="AX56" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="AY56" s="35">
+      <c r="AY56" s="33">
         <f>+Main!I7</f>
-        <v>92.37</v>
+        <v>99.56</v>
       </c>
     </row>
     <row r="57" spans="2:51" s="6" customFormat="1">
@@ -7627,56 +7637,56 @@
         <f>+SUM(V58:V59,V64)-SUM(V80:V81,V83)</f>
         <v>-11581.9</v>
       </c>
-      <c r="AK57" s="6">
-        <f>+T57</f>
-        <v>-11731.9</v>
-      </c>
       <c r="AL57" s="6">
-        <f>+AK57+AL44</f>
-        <v>-8450.1000000000022</v>
+        <f>+V57+AM44</f>
+        <v>-6675.5113012360962</v>
       </c>
       <c r="AM57" s="6">
-        <f t="shared" ref="AM57:AU57" si="131">+AL57+AM44</f>
-        <v>-3526.9839531962116</v>
+        <f t="shared" ref="AM57:AV57" si="131">+AL57+AM44</f>
+        <v>-1769.1226024721927</v>
       </c>
       <c r="AN57" s="6">
+        <f t="shared" ref="AN57" si="132">+AM57+AN44</f>
+        <v>3548.7690580467652</v>
+      </c>
+      <c r="AO57" s="6">
+        <f t="shared" ref="AO57" si="133">+AN57+AO44</f>
+        <v>9291.919492355466</v>
+      </c>
+      <c r="AP57" s="6">
+        <f t="shared" ref="AP57" si="134">+AO57+AP44</f>
+        <v>15474.494943315238</v>
+      </c>
+      <c r="AQ57" s="6">
+        <f t="shared" ref="AQ57" si="135">+AP57+AQ44</f>
+        <v>22111.082357416461</v>
+      </c>
+      <c r="AR57" s="6">
+        <f t="shared" ref="AR57" si="136">+AQ57+AR44</f>
+        <v>29216.699927659094</v>
+      </c>
+      <c r="AS57" s="6">
+        <f t="shared" ref="AS57" si="137">+AR57+AS44</f>
+        <v>36806.807912668242</v>
+      </c>
+      <c r="AT57" s="6">
+        <f t="shared" ref="AT57" si="138">+AS57+AT44</f>
+        <v>44897.319738362465</v>
+      </c>
+      <c r="AU57" s="6">
+        <f t="shared" ref="AU57" si="139">+AT57+AU44</f>
+        <v>53504.613388656944</v>
+      </c>
+      <c r="AV57" s="6">
         <f t="shared" si="131"/>
-        <v>1812.3679862362023</v>
-      </c>
-      <c r="AO57" s="6">
-        <f t="shared" si="131"/>
-        <v>7581.8578708951809</v>
-      </c>
-      <c r="AP57" s="6">
-        <f t="shared" si="131"/>
-        <v>13795.800685226182</v>
-      </c>
-      <c r="AQ57" s="6">
-        <f t="shared" si="131"/>
-        <v>20468.934601652043</v>
-      </c>
-      <c r="AR57" s="6">
-        <f t="shared" si="131"/>
-        <v>27616.431502784937</v>
-      </c>
-      <c r="AS57" s="6">
-        <f t="shared" si="131"/>
-        <v>35253.907775631065</v>
-      </c>
-      <c r="AT57" s="6">
-        <f t="shared" si="131"/>
-        <v>43397.435383847471</v>
-      </c>
-      <c r="AU57" s="6">
-        <f t="shared" si="131"/>
-        <v>52063.553224262316</v>
-      </c>
-      <c r="AX57" s="36" t="s">
+        <v>62645.543091851898</v>
+      </c>
+      <c r="AX57" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="AY57" s="37">
+      <c r="AY57" s="35">
         <f>+AY55/AY56-1</f>
-        <v>-6.5118766714620469E-2</v>
+        <v>-0.13869518763353217</v>
       </c>
     </row>
     <row r="58" spans="2:51">
@@ -7722,49 +7732,49 @@
       <c r="V58" s="14">
         <v>2818.4</v>
       </c>
-      <c r="AK58" s="4">
-        <f>+SUM(S58:S59)+S64+S65</f>
-        <v>4608.3</v>
-      </c>
       <c r="AL58" s="4">
-        <f>+AK58</f>
-        <v>4608.3</v>
+        <f>+V58</f>
+        <v>2818.4</v>
       </c>
       <c r="AM58" s="4">
-        <f>+AL58</f>
-        <v>4608.3</v>
+        <f>+AL58*(1+$AY$47)</f>
+        <v>2931.1360000000004</v>
       </c>
       <c r="AN58" s="4">
-        <f>+AM58</f>
-        <v>4608.3</v>
+        <f t="shared" ref="AN58:AV58" si="140">+AM58*(1+$AY$47)</f>
+        <v>3048.3814400000006</v>
       </c>
       <c r="AO58" s="4">
-        <f t="shared" ref="AO58:AU58" si="132">+AN58</f>
-        <v>4608.3</v>
+        <f t="shared" si="140"/>
+        <v>3170.3166976000007</v>
       </c>
       <c r="AP58" s="4">
-        <f t="shared" si="132"/>
-        <v>4608.3</v>
+        <f t="shared" si="140"/>
+        <v>3297.1293655040008</v>
       </c>
       <c r="AQ58" s="4">
-        <f t="shared" si="132"/>
-        <v>4608.3</v>
+        <f t="shared" si="140"/>
+        <v>3429.0145401241612</v>
       </c>
       <c r="AR58" s="4">
-        <f t="shared" si="132"/>
-        <v>4608.3</v>
+        <f t="shared" si="140"/>
+        <v>3566.1751217291276</v>
       </c>
       <c r="AS58" s="4">
-        <f t="shared" si="132"/>
-        <v>4608.3</v>
+        <f t="shared" si="140"/>
+        <v>3708.8221265982929</v>
       </c>
       <c r="AT58" s="4">
-        <f t="shared" si="132"/>
-        <v>4608.3</v>
+        <f t="shared" si="140"/>
+        <v>3857.1750116622247</v>
       </c>
       <c r="AU58" s="4">
-        <f t="shared" si="132"/>
-        <v>4608.3</v>
+        <f t="shared" si="140"/>
+        <v>4011.4620121287139</v>
+      </c>
+      <c r="AV58" s="4">
+        <f t="shared" si="140"/>
+        <v>4171.9204926138627</v>
       </c>
     </row>
     <row r="59" spans="2:51">
@@ -7955,55 +7965,55 @@
       <c r="H63" s="22"/>
       <c r="I63" s="22"/>
       <c r="J63" s="22">
-        <f t="shared" ref="J63:K63" si="133">+SUM(J58:J62)</f>
+        <f t="shared" ref="J63:K63" si="141">+SUM(J58:J62)</f>
         <v>5653.9000000000005</v>
       </c>
       <c r="K63" s="22">
-        <f t="shared" si="133"/>
+        <f t="shared" si="141"/>
         <v>5899.7</v>
       </c>
       <c r="L63" s="22">
-        <f t="shared" ref="L63:M63" si="134">+SUM(L58:L62)</f>
+        <f t="shared" ref="L63:M63" si="142">+SUM(L58:L62)</f>
         <v>5749.9000000000005</v>
       </c>
       <c r="M63" s="22">
-        <f t="shared" si="134"/>
+        <f t="shared" si="142"/>
         <v>7581.0000000000009</v>
       </c>
       <c r="N63" s="22">
-        <f t="shared" ref="N63:T63" si="135">+SUM(N58:N62)</f>
+        <f t="shared" ref="N63:T63" si="143">+SUM(N58:N62)</f>
         <v>7806.4</v>
       </c>
       <c r="O63" s="22">
-        <f t="shared" si="135"/>
+        <f t="shared" si="143"/>
         <v>8357.5</v>
       </c>
       <c r="P63" s="22">
-        <f t="shared" si="135"/>
+        <f t="shared" si="143"/>
         <v>6979.5</v>
       </c>
       <c r="Q63" s="22">
-        <f t="shared" si="135"/>
+        <f t="shared" si="143"/>
         <v>7931.7000000000007</v>
       </c>
       <c r="R63" s="22">
-        <f t="shared" si="135"/>
+        <f t="shared" si="143"/>
         <v>9756.4</v>
       </c>
       <c r="S63" s="22">
-        <f t="shared" si="135"/>
+        <f t="shared" si="143"/>
         <v>7255.1</v>
       </c>
       <c r="T63" s="22">
-        <f t="shared" si="135"/>
+        <f t="shared" si="143"/>
         <v>7541.0999999999995</v>
       </c>
       <c r="U63" s="22">
-        <f t="shared" ref="U63:V63" si="136">+SUM(U58:U62)</f>
+        <f t="shared" ref="U63:V63" si="144">+SUM(U58:U62)</f>
         <v>7067.5</v>
       </c>
       <c r="V63" s="22">
-        <f t="shared" si="136"/>
+        <f t="shared" si="144"/>
         <v>7018.7</v>
       </c>
     </row>
@@ -8371,55 +8381,55 @@
       <c r="H72" s="22"/>
       <c r="I72" s="22"/>
       <c r="J72" s="22">
-        <f t="shared" ref="J72:K72" si="137">+SUM(J63:J71)</f>
+        <f t="shared" ref="J72:K72" si="145">+SUM(J63:J71)</f>
         <v>19219.599999999999</v>
       </c>
       <c r="K72" s="22">
-        <f t="shared" si="137"/>
+        <f t="shared" si="145"/>
         <v>27731.300000000003</v>
       </c>
       <c r="L72" s="22">
-        <f t="shared" ref="L72:M72" si="138">+SUM(L63:L71)</f>
+        <f t="shared" ref="L72:M72" si="146">+SUM(L63:L71)</f>
         <v>27478.9</v>
       </c>
       <c r="M72" s="22">
-        <f t="shared" si="138"/>
+        <f t="shared" si="146"/>
         <v>29140.599999999995</v>
       </c>
       <c r="N72" s="22">
-        <f t="shared" ref="N72:T72" si="139">+SUM(N63:N71)</f>
+        <f t="shared" ref="N72:T72" si="147">+SUM(N63:N71)</f>
         <v>29374.5</v>
       </c>
       <c r="O72" s="22">
-        <f t="shared" si="139"/>
+        <f t="shared" si="147"/>
         <v>29968.399999999998</v>
       </c>
       <c r="P72" s="22">
-        <f t="shared" si="139"/>
+        <f t="shared" si="147"/>
         <v>28371.7</v>
       </c>
       <c r="Q72" s="22">
-        <f t="shared" si="139"/>
+        <f t="shared" si="147"/>
         <v>29476.799999999999</v>
       </c>
       <c r="R72" s="22">
-        <f t="shared" si="139"/>
+        <f t="shared" si="147"/>
         <v>31392.3</v>
       </c>
       <c r="S72" s="22">
-        <f t="shared" si="139"/>
+        <f t="shared" si="147"/>
         <v>28833.9</v>
       </c>
       <c r="T72" s="22">
-        <f t="shared" si="139"/>
+        <f t="shared" si="147"/>
         <v>29021.5</v>
       </c>
       <c r="U72" s="22">
-        <f t="shared" ref="U72:V72" si="140">+SUM(U63:U71)</f>
+        <f t="shared" ref="U72:V72" si="148">+SUM(U63:U71)</f>
         <v>28156.000000000007</v>
       </c>
       <c r="V72" s="22">
-        <f t="shared" si="140"/>
+        <f t="shared" si="148"/>
         <v>27978.400000000001</v>
       </c>
     </row>
@@ -8735,43 +8745,43 @@
         <v>200</v>
       </c>
       <c r="AL80" s="4">
-        <f t="shared" ref="AL80:AU80" si="141">AK80-(AK80*$AY$48)</f>
+        <f t="shared" ref="AL80:AU80" si="149">AK80-(AK80*$AY$48)</f>
         <v>194</v>
       </c>
       <c r="AM80" s="4">
-        <f t="shared" si="141"/>
+        <f t="shared" si="149"/>
         <v>188.18</v>
       </c>
       <c r="AN80" s="4">
-        <f t="shared" si="141"/>
+        <f t="shared" si="149"/>
         <v>182.53460000000001</v>
       </c>
       <c r="AO80" s="4">
-        <f t="shared" si="141"/>
+        <f t="shared" si="149"/>
         <v>177.05856200000002</v>
       </c>
       <c r="AP80" s="4">
-        <f t="shared" si="141"/>
+        <f t="shared" si="149"/>
         <v>171.74680514000002</v>
       </c>
       <c r="AQ80" s="4">
-        <f t="shared" si="141"/>
+        <f t="shared" si="149"/>
         <v>166.59440098580001</v>
       </c>
       <c r="AR80" s="4">
-        <f t="shared" si="141"/>
+        <f t="shared" si="149"/>
         <v>161.59656895622601</v>
       </c>
       <c r="AS80" s="4">
-        <f t="shared" si="141"/>
+        <f t="shared" si="149"/>
         <v>156.74867188753922</v>
       </c>
       <c r="AT80" s="4">
-        <f t="shared" si="141"/>
+        <f t="shared" si="149"/>
         <v>152.04621173091303</v>
       </c>
       <c r="AU80" s="4">
-        <f t="shared" si="141"/>
+        <f t="shared" si="149"/>
         <v>147.48482537898565</v>
       </c>
     </row>
@@ -8831,55 +8841,55 @@
       <c r="H82" s="22"/>
       <c r="I82" s="22"/>
       <c r="J82" s="22">
-        <f t="shared" ref="J82:K82" si="142">+SUM(J74:J81)</f>
+        <f t="shared" ref="J82:K82" si="150">+SUM(J74:J81)</f>
         <v>6168.7</v>
       </c>
       <c r="K82" s="22">
-        <f t="shared" si="142"/>
+        <f t="shared" si="150"/>
         <v>8675.5</v>
       </c>
       <c r="L82" s="22">
-        <f t="shared" ref="L82:M82" si="143">+SUM(L74:L81)</f>
+        <f t="shared" ref="L82:M82" si="151">+SUM(L74:L81)</f>
         <v>8265.7999999999993</v>
       </c>
       <c r="M82" s="22">
-        <f t="shared" si="143"/>
+        <f t="shared" si="151"/>
         <v>8002</v>
       </c>
       <c r="N82" s="22">
-        <f t="shared" ref="N82:T82" si="144">+SUM(N74:N81)</f>
+        <f t="shared" ref="N82:T82" si="152">+SUM(N74:N81)</f>
         <v>7346.7999999999993</v>
       </c>
       <c r="O82" s="22">
-        <f t="shared" si="144"/>
+        <f t="shared" si="152"/>
         <v>7883.9000000000005</v>
       </c>
       <c r="P82" s="22">
-        <f t="shared" si="144"/>
+        <f t="shared" si="152"/>
         <v>6505.0999999999995</v>
       </c>
       <c r="Q82" s="22">
-        <f t="shared" si="144"/>
+        <f t="shared" si="152"/>
         <v>7799.8</v>
       </c>
       <c r="R82" s="22">
-        <f t="shared" si="144"/>
+        <f t="shared" si="152"/>
         <v>8151.4</v>
       </c>
       <c r="S82" s="22">
-        <f t="shared" si="144"/>
+        <f t="shared" si="152"/>
         <v>8920.7000000000007</v>
       </c>
       <c r="T82" s="22">
-        <f t="shared" si="144"/>
+        <f t="shared" si="152"/>
         <v>9104.3000000000011</v>
       </c>
       <c r="U82" s="22">
-        <f t="shared" ref="U82:V82" si="145">+SUM(U74:U81)</f>
+        <f t="shared" ref="U82:V82" si="153">+SUM(U74:U81)</f>
         <v>8402.4</v>
       </c>
       <c r="V82" s="22">
-        <f t="shared" si="145"/>
+        <f t="shared" si="153"/>
         <v>9151.7999999999993</v>
       </c>
     </row>
@@ -8931,43 +8941,43 @@
         <v>13586.3</v>
       </c>
       <c r="AL83" s="4">
-        <f t="shared" ref="AL83:AU83" si="146">AK83-(AK83*$AY$48)</f>
+        <f t="shared" ref="AL83:AU83" si="154">AK83-(AK83*$AY$48)</f>
         <v>13178.710999999999</v>
       </c>
       <c r="AM83" s="4">
-        <f t="shared" si="146"/>
+        <f t="shared" si="154"/>
         <v>12783.34967</v>
       </c>
       <c r="AN83" s="4">
-        <f t="shared" si="146"/>
+        <f t="shared" si="154"/>
         <v>12399.8491799</v>
       </c>
       <c r="AO83" s="4">
-        <f t="shared" si="146"/>
+        <f t="shared" si="154"/>
         <v>12027.853704503001</v>
       </c>
       <c r="AP83" s="4">
-        <f t="shared" si="146"/>
+        <f t="shared" si="154"/>
         <v>11667.018093367911</v>
       </c>
       <c r="AQ83" s="4">
-        <f t="shared" si="146"/>
+        <f t="shared" si="154"/>
         <v>11317.007550566874</v>
       </c>
       <c r="AR83" s="4">
-        <f t="shared" si="146"/>
+        <f t="shared" si="154"/>
         <v>10977.497324049868</v>
       </c>
       <c r="AS83" s="4">
-        <f t="shared" si="146"/>
+        <f t="shared" si="154"/>
         <v>10648.172404328372</v>
       </c>
       <c r="AT83" s="4">
-        <f t="shared" si="146"/>
+        <f t="shared" si="154"/>
         <v>10328.72723219852</v>
       </c>
       <c r="AU83" s="4">
-        <f t="shared" si="146"/>
+        <f t="shared" si="154"/>
         <v>10018.865415232565</v>
       </c>
     </row>
@@ -9115,55 +9125,55 @@
       <c r="H87" s="22"/>
       <c r="I87" s="22"/>
       <c r="J87" s="22">
-        <f t="shared" ref="J87:K87" si="147">+SUM(J82:J86)</f>
+        <f t="shared" ref="J87:K87" si="155">+SUM(J82:J86)</f>
         <v>25450.6</v>
       </c>
       <c r="K87" s="22">
-        <f t="shared" si="147"/>
+        <f t="shared" si="155"/>
         <v>34490.400000000001</v>
       </c>
       <c r="L87" s="22">
-        <f t="shared" ref="L87:M87" si="148">+SUM(L82:L86)</f>
+        <f t="shared" ref="L87:M87" si="156">+SUM(L82:L86)</f>
         <v>35011.800000000003</v>
       </c>
       <c r="M87" s="22">
-        <f t="shared" si="148"/>
+        <f t="shared" si="156"/>
         <v>37764.899999999994</v>
       </c>
       <c r="N87" s="22">
-        <f t="shared" ref="N87:T87" si="149">+SUM(N82:N86)</f>
+        <f t="shared" ref="N87:T87" si="157">+SUM(N82:N86)</f>
         <v>37174.199999999997</v>
       </c>
       <c r="O87" s="22">
-        <f t="shared" si="149"/>
+        <f t="shared" si="157"/>
         <v>37872.400000000001</v>
       </c>
       <c r="P87" s="22">
-        <f t="shared" si="149"/>
+        <f t="shared" si="157"/>
         <v>36020</v>
       </c>
       <c r="Q87" s="22">
-        <f t="shared" si="149"/>
+        <f t="shared" si="157"/>
         <v>36271.1</v>
       </c>
       <c r="R87" s="22">
-        <f t="shared" si="149"/>
+        <f t="shared" si="157"/>
         <v>36707.100000000006</v>
       </c>
       <c r="S87" s="22">
-        <f t="shared" si="149"/>
+        <f t="shared" si="157"/>
         <v>37283.799999999996</v>
       </c>
       <c r="T87" s="22">
-        <f t="shared" si="149"/>
+        <f t="shared" si="157"/>
         <v>37782.699999999997</v>
       </c>
       <c r="U87" s="22">
-        <f t="shared" ref="U87:V87" si="150">+SUM(U82:U86)</f>
+        <f t="shared" ref="U87:V87" si="158">+SUM(U82:U86)</f>
         <v>26815.1</v>
       </c>
       <c r="V87" s="22">
-        <f t="shared" si="150"/>
+        <f t="shared" si="158"/>
         <v>36677.1</v>
       </c>
     </row>
@@ -9223,55 +9233,55 @@
       <c r="H89" s="22"/>
       <c r="I89" s="22"/>
       <c r="J89" s="22">
-        <f t="shared" ref="J89:K89" si="151">+J87+J88</f>
+        <f t="shared" ref="J89:K89" si="159">+J87+J88</f>
         <v>19219.599999999999</v>
       </c>
       <c r="K89" s="22">
-        <f t="shared" si="151"/>
+        <f t="shared" si="159"/>
         <v>27731.300000000003</v>
       </c>
       <c r="L89" s="22">
-        <f t="shared" ref="L89:M89" si="152">+L87+L88</f>
+        <f t="shared" ref="L89:M89" si="160">+L87+L88</f>
         <v>27478.9</v>
       </c>
       <c r="M89" s="22">
-        <f t="shared" si="152"/>
+        <f t="shared" si="160"/>
         <v>29140.599999999995</v>
       </c>
       <c r="N89" s="22">
-        <f t="shared" ref="N89:T89" si="153">+N87+N88</f>
+        <f t="shared" ref="N89:T89" si="161">+N87+N88</f>
         <v>29374.799999999996</v>
       </c>
       <c r="O89" s="22">
-        <f t="shared" si="153"/>
+        <f t="shared" si="161"/>
         <v>29968.400000000001</v>
       </c>
       <c r="P89" s="22">
-        <f t="shared" si="153"/>
+        <f t="shared" si="161"/>
         <v>28371.7</v>
       </c>
       <c r="Q89" s="22">
-        <f t="shared" si="153"/>
+        <f t="shared" si="161"/>
         <v>29476.799999999999</v>
       </c>
       <c r="R89" s="22">
-        <f t="shared" si="153"/>
+        <f t="shared" si="161"/>
         <v>31392.600000000006</v>
       </c>
       <c r="S89" s="22">
-        <f t="shared" si="153"/>
+        <f t="shared" si="161"/>
         <v>28833.499999999996</v>
       </c>
       <c r="T89" s="22">
-        <f t="shared" si="153"/>
+        <f t="shared" si="161"/>
         <v>29021.499999999996</v>
       </c>
       <c r="U89" s="22">
-        <f t="shared" ref="U89:V89" si="154">+U87+U88</f>
+        <f t="shared" ref="U89:V89" si="162">+U87+U88</f>
         <v>18156.199999999997</v>
       </c>
       <c r="V89" s="22">
-        <f t="shared" si="154"/>
+        <f t="shared" si="162"/>
         <v>27978.399999999998</v>
       </c>
     </row>
@@ -9321,35 +9331,35 @@
         <v>459.60000000000036</v>
       </c>
       <c r="O91" s="14">
-        <f t="shared" ref="O91:S91" si="155">+O63-O82</f>
+        <f t="shared" ref="O91:S91" si="163">+O63-O82</f>
         <v>473.59999999999945</v>
       </c>
       <c r="P91" s="14">
-        <f t="shared" si="155"/>
+        <f t="shared" si="163"/>
         <v>474.40000000000055</v>
       </c>
       <c r="Q91" s="14">
-        <f t="shared" si="155"/>
+        <f t="shared" si="163"/>
         <v>131.90000000000055</v>
       </c>
       <c r="R91" s="14">
-        <f t="shared" si="155"/>
+        <f t="shared" si="163"/>
         <v>1605</v>
       </c>
       <c r="S91" s="14">
-        <f t="shared" si="155"/>
+        <f t="shared" si="163"/>
         <v>-1665.6000000000004</v>
       </c>
       <c r="T91" s="14">
-        <f t="shared" ref="T91:U91" si="156">+T63-T82</f>
+        <f t="shared" ref="T91:U91" si="164">+T63-T82</f>
         <v>-1563.2000000000016</v>
       </c>
       <c r="U91" s="14">
-        <f t="shared" si="156"/>
+        <f t="shared" si="164"/>
         <v>-1334.8999999999996</v>
       </c>
       <c r="V91" s="14">
-        <f t="shared" ref="V91" si="157">+V63-V82</f>
+        <f t="shared" ref="V91" si="165">+V63-V82</f>
         <v>-2133.0999999999995</v>
       </c>
     </row>
@@ -9365,39 +9375,39 @@
       <c r="H92" s="26"/>
       <c r="I92" s="26"/>
       <c r="J92" s="28">
-        <f t="shared" ref="J92:R92" si="158">+J25/(SUM(I61:J61)/2)</f>
+        <f t="shared" ref="J92:R92" si="166">+J25/(SUM(I61:J61)/2)</f>
         <v>2.7979599843075711</v>
       </c>
       <c r="K92" s="28">
-        <f t="shared" si="158"/>
+        <f t="shared" si="166"/>
         <v>1.522344372213335</v>
       </c>
       <c r="L92" s="28">
-        <f t="shared" si="158"/>
+        <f t="shared" si="166"/>
         <v>1.3772967010238202</v>
       </c>
       <c r="M92" s="28">
-        <f t="shared" si="158"/>
+        <f t="shared" si="166"/>
         <v>0.96488946684005206</v>
       </c>
       <c r="N92" s="28">
-        <f t="shared" si="158"/>
+        <f t="shared" si="166"/>
         <v>1.2610359785659608</v>
       </c>
       <c r="O92" s="28">
-        <f t="shared" si="158"/>
+        <f t="shared" si="166"/>
         <v>1.3557180191207119</v>
       </c>
       <c r="P92" s="28">
-        <f t="shared" si="158"/>
+        <f t="shared" si="166"/>
         <v>1.3393835501327687</v>
       </c>
       <c r="Q92" s="28">
-        <f t="shared" si="158"/>
+        <f t="shared" si="166"/>
         <v>1.4457041745854904</v>
       </c>
       <c r="R92" s="28">
-        <f t="shared" si="158"/>
+        <f t="shared" si="166"/>
         <v>1.5805970622759429</v>
       </c>
       <c r="S92" s="28">
@@ -9422,39 +9432,39 @@
         <v>152</v>
       </c>
       <c r="J93" s="14">
-        <f t="shared" ref="J93:R93" si="159">+(J61/J25)*365</f>
+        <f t="shared" ref="J93:R93" si="167">+(J61/J25)*365</f>
         <v>260.90437464946717</v>
       </c>
       <c r="K93" s="14">
-        <f t="shared" si="159"/>
+        <f t="shared" si="167"/>
         <v>229.9121355750313</v>
       </c>
       <c r="L93" s="14">
-        <f t="shared" si="159"/>
+        <f t="shared" si="167"/>
         <v>272.64003604144767</v>
       </c>
       <c r="M93" s="14">
-        <f t="shared" si="159"/>
+        <f t="shared" si="167"/>
         <v>389.54649595687329</v>
       </c>
       <c r="N93" s="14">
-        <f t="shared" si="159"/>
+        <f t="shared" si="167"/>
         <v>286.45335896398223</v>
       </c>
       <c r="O93" s="14">
-        <f t="shared" si="159"/>
+        <f t="shared" si="167"/>
         <v>262.11385486311065</v>
       </c>
       <c r="P93" s="14">
-        <f t="shared" si="159"/>
+        <f t="shared" si="167"/>
         <v>275.45372415177673</v>
       </c>
       <c r="Q93" s="14">
-        <f t="shared" si="159"/>
+        <f t="shared" si="167"/>
         <v>256.16183136899366</v>
       </c>
       <c r="R93" s="14">
-        <f t="shared" si="159"/>
+        <f t="shared" si="167"/>
         <v>235.00602143631332</v>
       </c>
       <c r="S93" s="14">
@@ -9486,39 +9496,39 @@
       <c r="H94" s="23"/>
       <c r="I94" s="23"/>
       <c r="J94" s="23">
-        <f t="shared" ref="J94:R94" si="160">+SUM(G44:J44)/(SUM(I72:J72)/2)</f>
+        <f t="shared" ref="J94:R94" si="168">+SUM(G44:J44)/(SUM(I72:J72)/2)</f>
         <v>0.37456554767008682</v>
       </c>
       <c r="K94" s="23">
-        <f t="shared" si="160"/>
+        <f t="shared" si="168"/>
         <v>0.15865936542217504</v>
       </c>
       <c r="L94" s="23">
-        <f t="shared" si="160"/>
+        <f t="shared" si="168"/>
         <v>0.12279614998677779</v>
       </c>
       <c r="M94" s="23">
-        <f t="shared" si="160"/>
+        <f t="shared" si="168"/>
         <v>4.7284062911187794E-2</v>
       </c>
       <c r="N94" s="23">
-        <f t="shared" si="160"/>
+        <f t="shared" si="168"/>
         <v>3.1728562371080286E-2</v>
       </c>
       <c r="O94" s="23">
-        <f t="shared" si="160"/>
+        <f t="shared" si="168"/>
         <v>2.2405376211813054E-2</v>
       </c>
       <c r="P94" s="23">
-        <f t="shared" si="160"/>
+        <f t="shared" si="168"/>
         <v>3.413775430621481E-2</v>
       </c>
       <c r="Q94" s="23">
-        <f t="shared" si="160"/>
+        <f t="shared" si="168"/>
         <v>9.7758801006076299E-2</v>
       </c>
       <c r="R94" s="23">
-        <f t="shared" si="160"/>
+        <f t="shared" si="168"/>
         <v>0.13798134028595793</v>
       </c>
       <c r="S94" s="23">
@@ -9585,27 +9595,27 @@
         <v>15</v>
       </c>
       <c r="N97" s="23">
-        <f t="shared" ref="N97:N128" si="161">+N58/N$72</f>
+        <f t="shared" ref="N97:N128" si="169">+N58/N$72</f>
         <v>0.14811826584282284</v>
       </c>
       <c r="O97" s="23">
-        <f t="shared" ref="O97:S97" si="162">+O58/O$72</f>
+        <f t="shared" ref="O97:S97" si="170">+O58/O$72</f>
         <v>0.16778006166495377</v>
       </c>
       <c r="P97" s="23">
-        <f t="shared" si="162"/>
+        <f t="shared" si="170"/>
         <v>0.13678066524036275</v>
       </c>
       <c r="Q97" s="23">
-        <f t="shared" si="162"/>
+        <f t="shared" si="170"/>
         <v>0.16124884655050753</v>
       </c>
       <c r="R97" s="23">
-        <f t="shared" si="162"/>
+        <f t="shared" si="170"/>
         <v>0.20564597050869163</v>
       </c>
       <c r="S97" s="23">
-        <f t="shared" si="162"/>
+        <f t="shared" si="170"/>
         <v>0.1376643464810518</v>
       </c>
     </row>
@@ -9614,27 +9624,27 @@
         <v>66</v>
       </c>
       <c r="N98" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>9.5729289009174618E-3</v>
       </c>
       <c r="O98" s="23">
-        <f t="shared" ref="O98:S107" si="163">+O59/O$72</f>
+        <f t="shared" ref="O98:S107" si="171">+O59/O$72</f>
         <v>7.8582773855127401E-3</v>
       </c>
       <c r="P98" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>4.3353059562874271E-3</v>
       </c>
       <c r="Q98" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>5.2108777072138084E-3</v>
       </c>
       <c r="R98" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>5.1668721310639864E-3</v>
       </c>
       <c r="S98" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>3.0311543010137373E-3</v>
       </c>
     </row>
@@ -9643,27 +9653,27 @@
         <v>67</v>
       </c>
       <c r="N99" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>3.0073703382185228E-2</v>
       </c>
       <c r="O99" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>2.9631211542825112E-2</v>
       </c>
       <c r="P99" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>3.1023872379871493E-2</v>
       </c>
       <c r="Q99" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>3.0912446398523585E-2</v>
       </c>
       <c r="R99" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>2.9943648601727175E-2</v>
       </c>
       <c r="S99" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>3.5759990844110572E-2</v>
       </c>
     </row>
@@ -9672,27 +9682,27 @@
         <v>68</v>
       </c>
       <c r="N100" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>5.2814515991761568E-2</v>
       </c>
       <c r="O100" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>4.9101720478904452E-2</v>
       </c>
       <c r="P100" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>5.2996471836372155E-2</v>
       </c>
       <c r="Q100" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>5.2522661890028771E-2</v>
       </c>
       <c r="R100" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>5.1092146800330022E-2</v>
       </c>
       <c r="S100" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>5.6776918835121155E-2</v>
       </c>
     </row>
@@ -9701,27 +9711,27 @@
         <v>69</v>
       </c>
       <c r="N101" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>2.5174896593984579E-2</v>
       </c>
       <c r="O101" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>2.4505812789471577E-2</v>
       </c>
       <c r="P101" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>2.0865862814001275E-2</v>
       </c>
       <c r="Q101" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>1.9187971557292516E-2</v>
       </c>
       <c r="R101" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>1.8940950487858488E-2</v>
       </c>
       <c r="S101" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>1.8384609782235495E-2</v>
       </c>
     </row>
@@ -9730,27 +9740,27 @@
         <v>62</v>
       </c>
       <c r="N102" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>0.26575431071167166</v>
       </c>
       <c r="O102" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.27887708386166765</v>
       </c>
       <c r="P102" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.2460021782268951</v>
       </c>
       <c r="Q102" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.26908280410356622</v>
       </c>
       <c r="R102" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.31078958852967126</v>
       </c>
       <c r="S102" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.25161702024353277</v>
       </c>
     </row>
@@ -9759,27 +9769,27 @@
         <v>70</v>
       </c>
       <c r="N103" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>7.0162896389725782E-3</v>
       </c>
       <c r="O103" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>6.3700431120780566E-3</v>
       </c>
       <c r="P103" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>1.0038171840249263E-2</v>
       </c>
       <c r="Q103" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>9.6991532323725781E-3</v>
       </c>
       <c r="R103" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>8.9735380969218573E-3</v>
       </c>
       <c r="S103" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>1.0390547237799952E-2</v>
       </c>
     </row>
@@ -9788,27 +9798,27 @@
         <v>71</v>
       </c>
       <c r="N104" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>1.6296447599108071E-2</v>
       </c>
       <c r="O104" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>1.6550766807704117E-2</v>
       </c>
       <c r="P104" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>1.7602047110324724E-2</v>
       </c>
       <c r="Q104" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>1.8160044509580416E-2</v>
       </c>
       <c r="R104" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>8.5530528186848372E-3</v>
       </c>
       <c r="S104" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>8.7362444899926825E-3</v>
       </c>
     </row>
@@ -9817,27 +9827,27 @@
         <v>72</v>
       </c>
       <c r="N105" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>0.21247680811588282</v>
       </c>
       <c r="O105" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.20614714165587752</v>
       </c>
       <c r="P105" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.21581716992637029</v>
       </c>
       <c r="Q105" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.20868615317809258</v>
       </c>
       <c r="R105" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.20290007422202261</v>
       </c>
       <c r="S105" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.22189159288198959</v>
       </c>
     </row>
@@ -9846,27 +9856,27 @@
         <v>73</v>
       </c>
       <c r="N106" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>0.27691024528077074</v>
       </c>
       <c r="O106" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.27360152694171197</v>
       </c>
       <c r="P106" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.28326818625602274</v>
       </c>
       <c r="Q106" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.27361178961081256</v>
       </c>
       <c r="R106" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.26235732966364361</v>
       </c>
       <c r="S106" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>0.28450539122352508</v>
       </c>
     </row>
@@ -9875,27 +9885,27 @@
         <v>74</v>
       </c>
       <c r="N107" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>6.093380312856389E-2</v>
       </c>
       <c r="O107" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>5.9809666181711407E-2</v>
       </c>
       <c r="P107" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>6.2386110102672733E-2</v>
       </c>
       <c r="Q107" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>6.2795147370135154E-2</v>
       </c>
       <c r="R107" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>5.9712095004188927E-2</v>
       </c>
       <c r="S107" s="23">
-        <f t="shared" si="163"/>
+        <f t="shared" si="171"/>
         <v>6.4496998324888408E-2</v>
       </c>
     </row>
@@ -9904,27 +9914,27 @@
         <v>75</v>
       </c>
       <c r="N108" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>1.9356925224259136E-2</v>
       </c>
       <c r="O108" s="23">
-        <f t="shared" ref="O108:S117" si="164">+O69/O$72</f>
+        <f t="shared" ref="O108:S117" si="172">+O69/O$72</f>
         <v>1.8055685321872374E-2</v>
       </c>
       <c r="P108" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>2.0263149546907656E-2</v>
       </c>
       <c r="Q108" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>1.989021874830375E-2</v>
       </c>
       <c r="R108" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>1.8428085868190607E-2</v>
       </c>
       <c r="S108" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>2.0392662803158781E-2</v>
       </c>
     </row>
@@ -9933,27 +9943,27 @@
         <v>76</v>
       </c>
       <c r="N109" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>1.879521353554954E-2</v>
       </c>
       <c r="O109" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>1.6897799014962429E-2</v>
       </c>
       <c r="P109" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>1.5659971027467513E-2</v>
       </c>
       <c r="Q109" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>1.3502144059056614E-2</v>
       </c>
       <c r="R109" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>1.1146045367813126E-2</v>
       </c>
       <c r="S109" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>1.0491123295842741E-2</v>
       </c>
     </row>
@@ -9962,27 +9972,27 @@
         <v>77</v>
       </c>
       <c r="N110" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>0.12245995676522153</v>
       </c>
       <c r="O110" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>0.12369028710241456</v>
       </c>
       <c r="P110" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>0.12896301596308998</v>
       </c>
       <c r="Q110" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>0.12457254518808011</v>
       </c>
       <c r="R110" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>0.11714019042886313</v>
       </c>
       <c r="S110" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>0.12747841949926994</v>
       </c>
     </row>
@@ -9991,53 +10001,53 @@
         <v>63</v>
       </c>
       <c r="N111" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>1</v>
       </c>
       <c r="O111" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>1</v>
       </c>
       <c r="P111" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>1</v>
       </c>
       <c r="Q111" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>1</v>
       </c>
       <c r="R111" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>1</v>
       </c>
       <c r="S111" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>1</v>
       </c>
     </row>
     <row r="112" spans="2:19" hidden="1" outlineLevel="1">
       <c r="N112" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>0</v>
       </c>
       <c r="O112" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>0</v>
       </c>
       <c r="P112" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>0</v>
       </c>
       <c r="Q112" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>0</v>
       </c>
       <c r="R112" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>0</v>
       </c>
       <c r="S112" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>0</v>
       </c>
     </row>
@@ -10046,27 +10056,27 @@
         <v>78</v>
       </c>
       <c r="N113" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>3.3971642070503329E-2</v>
       </c>
       <c r="O113" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>3.5056926629382951E-2</v>
       </c>
       <c r="P113" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>3.6430668588769789E-2</v>
       </c>
       <c r="Q113" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>3.8233458177278405E-2</v>
       </c>
       <c r="R113" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>3.8595451750907069E-2</v>
       </c>
       <c r="S113" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>4.47181962897839E-2</v>
       </c>
     </row>
@@ -10075,27 +10085,27 @@
         <v>79</v>
       </c>
       <c r="N114" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>3.9513864065771336E-2</v>
       </c>
       <c r="O114" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>5.3953497684227393E-2</v>
       </c>
       <c r="P114" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>6.2442504326494355E-2</v>
       </c>
       <c r="Q114" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>6.0773218259783969E-2</v>
       </c>
       <c r="R114" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>6.2856178107370278E-2</v>
       </c>
       <c r="S114" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>8.4771744370341851E-2</v>
       </c>
     </row>
@@ -10104,27 +10114,27 @@
         <v>80</v>
       </c>
       <c r="N115" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>2.3694020323750193E-2</v>
       </c>
       <c r="O115" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>2.2867420349434738E-2</v>
       </c>
       <c r="P115" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>2.2772692506969974E-2</v>
       </c>
       <c r="Q115" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>2.5138413939097867E-2</v>
       </c>
       <c r="R115" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>2.4601574271397763E-2</v>
       </c>
       <c r="S115" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>2.303191729179889E-2</v>
       </c>
     </row>
@@ -10133,27 +10143,27 @@
         <v>118</v>
       </c>
       <c r="N116" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>3.3430356261383173E-3</v>
       </c>
       <c r="O116" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>4.9952616756316652E-3</v>
       </c>
       <c r="P116" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>4.1238276169563333E-3</v>
       </c>
       <c r="Q116" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>6.947836942951746E-3</v>
       </c>
       <c r="R116" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>0</v>
       </c>
       <c r="S116" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>0</v>
       </c>
     </row>
@@ -10162,27 +10172,27 @@
         <v>81</v>
       </c>
       <c r="N117" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>4.2513064052154076E-2</v>
       </c>
       <c r="O117" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>4.22978871077535E-2</v>
       </c>
       <c r="P117" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>4.5693419851471712E-2</v>
       </c>
       <c r="Q117" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>4.4387450469521798E-2</v>
       </c>
       <c r="R117" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>1.1085520971703252E-2</v>
       </c>
       <c r="S117" s="23">
-        <f t="shared" si="164"/>
+        <f t="shared" si="172"/>
         <v>4.3466197774147786E-2</v>
       </c>
     </row>
@@ -10191,27 +10201,27 @@
         <v>82</v>
       </c>
       <c r="N118" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>4.9583822703365164E-2</v>
       </c>
       <c r="O118" s="23">
-        <f t="shared" ref="O118:S127" si="165">+O79/O$72</f>
+        <f t="shared" ref="O118:S127" si="173">+O79/O$72</f>
         <v>6.2439102521322468E-2</v>
       </c>
       <c r="P118" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>5.7173169038161262E-2</v>
       </c>
       <c r="Q118" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>5.5240053194376595E-2</v>
       </c>
       <c r="R118" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>3.9860093080150226E-2</v>
       </c>
       <c r="S118" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>7.181477358248449E-2</v>
       </c>
     </row>
@@ -10220,27 +10230,27 @@
         <v>83</v>
       </c>
       <c r="N119" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>1.4938126606410322E-2</v>
       </c>
       <c r="O119" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>1.6437313970715822E-2</v>
       </c>
       <c r="P119" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>6.4500893495983674E-4</v>
       </c>
       <c r="Q119" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0</v>
       </c>
       <c r="R119" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>5.0843678226826325E-2</v>
       </c>
       <c r="S119" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>6.9362798650199932E-3</v>
       </c>
     </row>
@@ -10249,27 +10259,27 @@
         <v>84</v>
       </c>
       <c r="N120" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>4.2550511498068058E-2</v>
       </c>
       <c r="O120" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>2.5026361100359048E-2</v>
       </c>
       <c r="P120" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0</v>
       </c>
       <c r="Q120" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>3.3887667589426261E-2</v>
       </c>
       <c r="R120" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>3.1819904881133274E-2</v>
       </c>
       <c r="S120" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>3.4643249785842357E-2</v>
       </c>
     </row>
@@ -10278,27 +10288,27 @@
         <v>61</v>
       </c>
       <c r="N121" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>0.25010808694616077</v>
       </c>
       <c r="O121" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.26307377103882762</v>
       </c>
       <c r="P121" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.22928129086378324</v>
       </c>
       <c r="Q121" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.26460809857243667</v>
       </c>
       <c r="R121" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.2596624012894882</v>
       </c>
       <c r="S121" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.30938235895941929</v>
       </c>
     </row>
@@ -10307,27 +10317,27 @@
         <v>85</v>
       </c>
       <c r="N122" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>0.49906892032204803</v>
       </c>
       <c r="O122" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.48963241280815795</v>
       </c>
       <c r="P122" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.51566525798595075</v>
       </c>
       <c r="Q122" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.46203115670629108</v>
       </c>
       <c r="R122" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.43376560494133909</v>
       </c>
       <c r="S122" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.47119189565060565</v>
       </c>
     </row>
@@ -10336,27 +10346,27 @@
         <v>86</v>
       </c>
       <c r="N123" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>0.26082826941735177</v>
       </c>
       <c r="O123" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.25875588953697898</v>
       </c>
       <c r="P123" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.26708656865820518</v>
       </c>
       <c r="Q123" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.2577552515876893</v>
       </c>
       <c r="R123" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.24649356689379243</v>
       </c>
       <c r="S123" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.26732422599787053</v>
       </c>
     </row>
@@ -10365,27 +10375,27 @@
         <v>87</v>
       </c>
       <c r="N124" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>0.22463361078486443</v>
       </c>
       <c r="O124" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.22015523017578517</v>
       </c>
       <c r="P124" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.23023294339077321</v>
       </c>
       <c r="Q124" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.22022064810291483</v>
       </c>
       <c r="R124" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.20587851160953483</v>
       </c>
       <c r="S124" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>0.22361525842844707</v>
       </c>
     </row>
@@ -10394,27 +10404,27 @@
         <v>88</v>
       </c>
       <c r="N125" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>3.0887334252497914E-2</v>
       </c>
       <c r="O125" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>3.2127173956567584E-2</v>
       </c>
       <c r="P125" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>2.7308902885621936E-2</v>
       </c>
       <c r="Q125" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>2.588137111219671E-2</v>
       </c>
       <c r="R125" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>2.3502578657823733E-2</v>
       </c>
       <c r="S125" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>2.1540617120819592E-2</v>
       </c>
     </row>
@@ -10423,27 +10433,27 @@
         <v>60</v>
       </c>
       <c r="N126" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>1.2655262217229228</v>
       </c>
       <c r="O126" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>1.2637444775163174</v>
       </c>
       <c r="P126" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>1.2695749637843343</v>
       </c>
       <c r="Q126" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>1.2304965260815286</v>
       </c>
       <c r="R126" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>1.1693026633919785</v>
       </c>
       <c r="S126" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>1.2930543561571619</v>
       </c>
     </row>
@@ -10452,27 +10462,27 @@
         <v>59</v>
       </c>
       <c r="N127" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>-0.2655160087831282</v>
       </c>
       <c r="O127" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>-0.26374447751631719</v>
       </c>
       <c r="P127" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>-0.26957496378433438</v>
       </c>
       <c r="Q127" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>-0.23049652608152854</v>
       </c>
       <c r="R127" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>-0.16929310690838201</v>
       </c>
       <c r="S127" s="23">
-        <f t="shared" si="165"/>
+        <f t="shared" si="173"/>
         <v>-0.29306822871689225</v>
       </c>
     </row>
@@ -10481,27 +10491,27 @@
         <v>58</v>
       </c>
       <c r="N128" s="23">
-        <f t="shared" si="161"/>
+        <f t="shared" si="169"/>
         <v>1.0000102129397945</v>
       </c>
       <c r="O128" s="23">
-        <f t="shared" ref="O128:S128" si="166">+O89/O$72</f>
+        <f t="shared" ref="O128:S128" si="174">+O89/O$72</f>
         <v>1.0000000000000002</v>
       </c>
       <c r="P128" s="23">
-        <f t="shared" si="166"/>
+        <f t="shared" si="174"/>
         <v>1</v>
       </c>
       <c r="Q128" s="23">
-        <f t="shared" si="166"/>
+        <f t="shared" si="174"/>
         <v>1</v>
       </c>
       <c r="R128" s="23">
-        <f t="shared" si="166"/>
+        <f t="shared" si="174"/>
         <v>1.0000095564835965</v>
       </c>
       <c r="S128" s="23">
-        <f t="shared" si="166"/>
+        <f t="shared" si="174"/>
         <v>0.99998612744026982</v>
       </c>
     </row>
@@ -11440,15 +11450,15 @@
       <c r="M169" s="22"/>
       <c r="N169" s="22"/>
       <c r="O169" s="22">
-        <f t="shared" ref="O169:Q169" si="167">+O148+O153+O136</f>
+        <f t="shared" ref="O169:Q169" si="175">+O148+O153+O136</f>
         <v>1610.7999999999997</v>
       </c>
       <c r="P169" s="22">
-        <f t="shared" si="167"/>
+        <f t="shared" si="175"/>
         <v>596.09999999999991</v>
       </c>
       <c r="Q169" s="22">
-        <f t="shared" si="167"/>
+        <f t="shared" si="175"/>
         <v>1402.1999999999998</v>
       </c>
       <c r="R169" s="22">
@@ -11466,11 +11476,11 @@
         <v>9711.1</v>
       </c>
       <c r="AI169" s="6">
-        <f t="shared" ref="AI169:AJ169" si="168">+AI148+AI153-AI137</f>
+        <f t="shared" ref="AI169:AJ169" si="176">+AI148+AI153-AI137</f>
         <v>2932.4</v>
       </c>
       <c r="AJ169" s="6">
-        <f t="shared" si="168"/>
+        <f t="shared" si="176"/>
         <v>-134.39999999999995</v>
       </c>
       <c r="AK169" s="6">
@@ -11487,19 +11497,19 @@
         <v>90</v>
       </c>
       <c r="O170" s="14">
-        <f t="shared" ref="O170:R170" si="169">+O44</f>
+        <f t="shared" ref="O170:R170" si="177">+O44</f>
         <v>622.20000000000016</v>
       </c>
       <c r="P170" s="14">
-        <f t="shared" si="169"/>
+        <f t="shared" si="177"/>
         <v>659.4</v>
       </c>
       <c r="Q170" s="14">
-        <f t="shared" si="169"/>
+        <f t="shared" si="177"/>
         <v>1153.4000000000008</v>
       </c>
       <c r="R170" s="14">
-        <f t="shared" si="169"/>
+        <f t="shared" si="177"/>
         <v>1764.3999999999999</v>
       </c>
       <c r="S170" s="14">
@@ -11507,19 +11517,19 @@
         <v>816.10000000000014</v>
       </c>
       <c r="AH170" s="4">
-        <f t="shared" ref="AH170:AK170" si="170">+AH44</f>
+        <f t="shared" ref="AH170:AK170" si="178">+AH44</f>
         <v>4517.6199999999944</v>
       </c>
       <c r="AI170" s="4">
-        <f t="shared" si="170"/>
+        <f t="shared" si="178"/>
         <v>3599.5</v>
       </c>
       <c r="AJ170" s="4">
-        <f t="shared" si="170"/>
+        <f t="shared" si="178"/>
         <v>928.3</v>
       </c>
       <c r="AK170" s="4">
-        <f t="shared" si="170"/>
+        <f t="shared" si="178"/>
         <v>4199.4000000000005</v>
       </c>
       <c r="AL170" s="4">
@@ -11532,7 +11542,7 @@
         <v>147</v>
       </c>
       <c r="R172" s="14">
-        <f t="shared" ref="R172:R173" si="171">+SUM(O169:R169)</f>
+        <f t="shared" ref="R172:R173" si="179">+SUM(O169:R169)</f>
         <v>4552.0999999999995</v>
       </c>
       <c r="S172" s="14">
@@ -11545,7 +11555,7 @@
         <v>148</v>
       </c>
       <c r="R173" s="14">
-        <f t="shared" si="171"/>
+        <f t="shared" si="179"/>
         <v>4199.4000000000005</v>
       </c>
       <c r="S173" s="14">
@@ -11554,6 +11564,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="AY57">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="AI25:AK27 AI38:AK43 AI21:AK23 N57:R57 AI32:AK34 AI36:AK36 AI28:AK30 F32 I57:K57 M57 L57 C32:E32 J92:S92" formulaRange="1"/>

</xml_diff>